<commit_message>
fix a bug about false positives
</commit_message>
<xml_diff>
--- a/frequency.xlsx
+++ b/frequency.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14370" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="407">
   <si>
     <t>sys.stderr-&gt;getvalue</t>
   </si>
@@ -1210,6 +1210,36 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>sys._getframe-&gt;f_restricted</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;service_pack_major</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;major</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;minor</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;product_type</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;suite_mask</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;service_pack_minor</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;service_pack</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;platform</t>
+  </si>
+  <si>
+    <t>sys.getwindowsversion-&gt;build</t>
   </si>
 </sst>
 </file>
@@ -1576,18 +1606,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>394</v>
       </c>
@@ -1595,7 +1628,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1611,8 +1644,17 @@
       <c r="E2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1628,8 +1670,17 @@
       <c r="E3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1645,8 +1696,17 @@
       <c r="E4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1656,8 +1716,17 @@
       <c r="C5" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1667,8 +1736,17 @@
       <c r="C6" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1684,8 +1762,17 @@
       <c r="E7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7">
+        <v>67</v>
+      </c>
+      <c r="J7" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -1695,8 +1782,17 @@
       <c r="C8" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8">
+        <v>109</v>
+      </c>
+      <c r="J8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1706,8 +1802,17 @@
       <c r="C9" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9">
+        <v>221</v>
+      </c>
+      <c r="J9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1717,8 +1822,17 @@
       <c r="C10" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1728,8 +1842,17 @@
       <c r="C11" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1739,8 +1862,17 @@
       <c r="C12" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>213</v>
+      </c>
+      <c r="J12" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1750,8 +1882,17 @@
       <c r="C13" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>397</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1761,8 +1902,17 @@
       <c r="C14" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1772,8 +1922,17 @@
       <c r="C15" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -1783,8 +1942,17 @@
       <c r="C16" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1794,8 +1962,17 @@
       <c r="C17" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1805,8 +1982,17 @@
       <c r="C18" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
+      </c>
+      <c r="J18" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1816,8 +2002,17 @@
       <c r="C19" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="J19" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1827,8 +2022,17 @@
       <c r="C20" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1838,8 +2042,17 @@
       <c r="C21" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1849,8 +2062,17 @@
       <c r="C22" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1860,8 +2082,17 @@
       <c r="C23" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23">
+        <v>24</v>
+      </c>
+      <c r="J23" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1871,8 +2102,17 @@
       <c r="C24" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1888,8 +2128,14 @@
       <c r="E25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1899,8 +2145,17 @@
       <c r="C26" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1910,8 +2165,17 @@
       <c r="C27" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -1921,8 +2185,17 @@
       <c r="C28" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1932,8 +2205,17 @@
       <c r="C29" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1943,8 +2225,14 @@
       <c r="C30" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>406</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1960,8 +2248,14 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>399</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1977,8 +2271,14 @@
       <c r="E32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>400</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -1988,8 +2288,14 @@
       <c r="C33" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>405</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -1999,8 +2305,14 @@
       <c r="C34" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>401</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -2010,8 +2322,14 @@
       <c r="C35" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>404</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -2021,8 +2339,14 @@
       <c r="C36" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>398</v>
+      </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -2032,8 +2356,14 @@
       <c r="C37" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>403</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2043,8 +2373,14 @@
       <c r="C38" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>402</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -2054,8 +2390,17 @@
       <c r="C39" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>94</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -2065,8 +2410,17 @@
       <c r="C40" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -2076,8 +2430,17 @@
       <c r="C41" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -2087,8 +2450,17 @@
       <c r="C42" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -2098,8 +2470,17 @@
       <c r="C43" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>70</v>
+      </c>
+      <c r="I43">
+        <v>7</v>
+      </c>
+      <c r="J43" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2109,8 +2490,17 @@
       <c r="C44" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>61</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>73</v>
       </c>
@@ -2120,16 +2510,34 @@
       <c r="C45" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>96</v>
+      </c>
+      <c r="I45">
+        <v>21</v>
+      </c>
+      <c r="J45" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>76</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>34</v>
+      </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
+      <c r="J46" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2145,8 +2553,17 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>79</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -2162,8 +2579,17 @@
       <c r="E48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>84</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
+      </c>
+      <c r="J48" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -2173,8 +2599,17 @@
       <c r="C49" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2190,8 +2625,17 @@
       <c r="E50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50">
+        <v>14</v>
+      </c>
+      <c r="J50" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -2207,8 +2651,17 @@
       <c r="E51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2218,8 +2671,17 @@
       <c r="C52" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
+      <c r="J52" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -2229,8 +2691,17 @@
       <c r="C53" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>47</v>
+      </c>
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="J53" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -2246,8 +2717,17 @@
       <c r="E54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54">
+        <v>5</v>
+      </c>
+      <c r="J54" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -2257,8 +2737,17 @@
       <c r="C55" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>60</v>
+      </c>
+      <c r="I55">
+        <v>4</v>
+      </c>
+      <c r="J55" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -2268,8 +2757,17 @@
       <c r="C56" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -2279,8 +2777,17 @@
       <c r="C57" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>43</v>
+      </c>
+      <c r="J57" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -2290,8 +2797,17 @@
       <c r="C58" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>92</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2301,8 +2817,17 @@
       <c r="C59" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>68</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>96</v>
       </c>
@@ -2312,8 +2837,17 @@
       <c r="C60" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>69</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2323,8 +2857,17 @@
       <c r="C61" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>51</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -2334,8 +2877,17 @@
       <c r="C62" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62">
+        <v>17</v>
+      </c>
+      <c r="J62" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -2345,8 +2897,17 @@
       <c r="C63" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I63">
+        <v>6</v>
+      </c>
+      <c r="J63" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -2356,8 +2917,17 @@
       <c r="C64" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>10</v>
+      </c>
+      <c r="I64">
+        <v>9</v>
+      </c>
+      <c r="J64" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -2373,8 +2943,17 @@
       <c r="E65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>56</v>
+      </c>
+      <c r="I65">
+        <v>7</v>
+      </c>
+      <c r="J65" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -2390,8 +2969,17 @@
       <c r="E66">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>48</v>
+      </c>
+      <c r="I66">
+        <v>4</v>
+      </c>
+      <c r="J66" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -2401,8 +2989,17 @@
       <c r="C67" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>89</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -2412,8 +3009,17 @@
       <c r="C68" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>7</v>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+      <c r="J68" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -2423,8 +3029,17 @@
       <c r="C69" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>93</v>
+      </c>
+      <c r="I69">
+        <v>20</v>
+      </c>
+      <c r="J69" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>21</v>
       </c>
@@ -2434,8 +3049,17 @@
       <c r="C70" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>99</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -2445,8 +3069,17 @@
       <c r="C71" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>67</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -2456,8 +3089,17 @@
       <c r="C72" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>41</v>
+      </c>
+      <c r="I72">
+        <v>17</v>
+      </c>
+      <c r="J72" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -2467,8 +3109,17 @@
       <c r="C73" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73">
+        <v>21</v>
+      </c>
+      <c r="J73" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>92</v>
       </c>
@@ -2478,8 +3129,17 @@
       <c r="C74" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>45</v>
+      </c>
+      <c r="I74">
+        <v>31</v>
+      </c>
+      <c r="J74" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>68</v>
       </c>
@@ -2489,8 +3149,17 @@
       <c r="C75" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>24</v>
+      </c>
+      <c r="I75">
+        <v>92</v>
+      </c>
+      <c r="J75" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>69</v>
       </c>
@@ -2500,8 +3169,17 @@
       <c r="C76" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>23</v>
+      </c>
+      <c r="I76">
+        <v>3</v>
+      </c>
+      <c r="J76" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>51</v>
       </c>
@@ -2511,8 +3189,17 @@
       <c r="C77" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>55</v>
+      </c>
+      <c r="I77">
+        <v>4</v>
+      </c>
+      <c r="J77" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2522,8 +3209,17 @@
       <c r="C78" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>53</v>
+      </c>
+      <c r="I78">
+        <v>7</v>
+      </c>
+      <c r="J78" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -2539,8 +3235,17 @@
       <c r="E79">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>83</v>
+      </c>
+      <c r="I79">
+        <v>14</v>
+      </c>
+      <c r="J79" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -2550,8 +3255,17 @@
       <c r="C80" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>81</v>
+      </c>
+      <c r="I80">
+        <v>10</v>
+      </c>
+      <c r="J80" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -2561,8 +3275,17 @@
       <c r="C81" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>11</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>56</v>
       </c>
@@ -2572,8 +3295,17 @@
       <c r="C82" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>95</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2583,8 +3315,17 @@
       <c r="C83" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>74</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -2594,8 +3335,17 @@
       <c r="C84" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>39</v>
+      </c>
+      <c r="I84">
+        <v>47</v>
+      </c>
+      <c r="J84" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -2606,7 +3356,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -2623,7 +3373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -2634,7 +3384,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -2645,7 +3395,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>99</v>
       </c>
@@ -2656,7 +3406,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>67</v>
       </c>
@@ -2667,7 +3417,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>41</v>
       </c>
@@ -2678,7 +3428,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -2689,7 +3439,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>45</v>
       </c>
@@ -2700,7 +3450,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -2711,7 +3461,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>23</v>
       </c>
@@ -2722,7 +3472,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>55</v>
       </c>
@@ -2811,8 +3561,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B103">
-    <sortCondition ref="A1:A103"/>
+  <sortState ref="H2:I84">
+    <sortCondition ref="H1:H83"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2822,7 +3572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>